<commit_message>
junit basic structure and billing server test
</commit_message>
<xml_diff>
--- a/Timetable/Krepela.xlsx
+++ b/Timetable/Krepela.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>class diagramm</t>
+  </si>
+  <si>
+    <t>src generated, libs added, create pricesteps</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
   <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -585,7 +588,7 @@
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -631,12 +634,21 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="6">
+        <v>41681</v>
+      </c>
+      <c r="B3" s="12">
+        <v>0.4375</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="D3" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="2"/>

</xml_diff>

<commit_message>
timetable: worked time added
</commit_message>
<xml_diff>
--- a/Timetable/Krepela.xlsx
+++ b/Timetable/Krepela.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>date</t>
   </si>
@@ -37,7 +37,10 @@
     <t>class diagramm</t>
   </si>
   <si>
-    <t>src generated, libs added, create pricesteps</t>
+    <t>billing server secure all functions</t>
+  </si>
+  <si>
+    <t>src generated, libs added, create pricesteps,  own exceptions</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
   <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -648,20 +651,28 @@
         <v>0.14583333333333337</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="6">
+        <v>41682</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="D4" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="2"/>
     </row>

</xml_diff>

<commit_message>
Changed Bill inner structure, added new class BillingLine
</commit_message>
<xml_diff>
--- a/Timetable/Krepela.xlsx
+++ b/Timetable/Krepela.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>src generated, libs added, create pricesteps,  own exceptions</t>
+  </si>
+  <si>
+    <t>Unittests,Bugfix, Pricesteps sortieren</t>
   </si>
 </sst>
 </file>
@@ -677,14 +680,22 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="6">
+        <v>41690</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0.4375</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.5</v>
+      </c>
       <c r="D5" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="2"/>
     </row>

</xml_diff>

<commit_message>
documentation persistence and timetable
</commit_message>
<xml_diff>
--- a/Timetable/Krepela.xlsx
+++ b/Timetable/Krepela.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Unittests,Bugfix, Pricesteps sortieren</t>
+  </si>
+  <si>
+    <t>Last controls and bugfixes</t>
   </si>
 </sst>
 </file>
@@ -585,7 +588,7 @@
   <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -700,14 +703,22 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="A6" s="6">
+        <v>41695</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>0.15972222222222215</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="2"/>
     </row>

</xml_diff>